<commit_message>
updates P supplementation and 2017 population estimates
</commit_message>
<xml_diff>
--- a/RawData/DGSalloc_master.xlsx
+++ b/RawData/DGSalloc_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N&amp;P/NANI_NAPI/NANI_NAPI_R/RawData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N_P/NANI_NAPI/CSNAPNIv1/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E963A274-E86B-AF4B-8E97-802E9FFE6820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB076392-47F0-7040-8A31-481E1317428D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="460" windowWidth="33600" windowHeight="19700" activeTab="2" xr2:uid="{DE6B0421-2367-3D4F-A0F9-F9ED10D5087D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19700" activeTab="5" xr2:uid="{DE6B0421-2367-3D4F-A0F9-F9ED10D5087D}"/>
   </bookViews>
   <sheets>
     <sheet name="replacement" sheetId="1" r:id="rId1"/>
@@ -911,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D9C13D-DDDC-734C-89A8-680426E92EDF}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
@@ -3088,105 +3088,102 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C28FF2F-89E4-4E4A-AB08-0C04C1DE0C75}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1">
-        <v>1987</v>
+        <v>1997</v>
       </c>
       <c r="C1">
-        <v>1992</v>
+        <v>2002</v>
       </c>
       <c r="D1">
-        <v>1997</v>
+        <v>2007</v>
       </c>
       <c r="E1">
-        <v>2002</v>
+        <v>2012</v>
       </c>
       <c r="F1">
-        <v>2007</v>
-      </c>
-      <c r="G1">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3218,15 +3215,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAE7606-04F6-8443-9766-C21E53844877}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>33.200000000000003</v>
       </c>
@@ -3234,19 +3231,16 @@
         <v>33.200000000000003</v>
       </c>
       <c r="C1">
-        <v>33.200000000000003</v>
+        <v>33.6</v>
       </c>
       <c r="D1">
-        <v>33.200000000000003</v>
+        <v>33</v>
       </c>
       <c r="E1">
-        <v>33.6</v>
-      </c>
-      <c r="F1">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24.5</v>
       </c>
@@ -3254,19 +3248,16 @@
         <v>24.5</v>
       </c>
       <c r="C2">
-        <v>24.5</v>
+        <v>24.4</v>
       </c>
       <c r="D2">
-        <v>24.5</v>
+        <v>25.4</v>
       </c>
       <c r="E2">
-        <v>24.4</v>
-      </c>
-      <c r="F2">
         <v>25.4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2.2000000000000002</v>
       </c>
@@ -3277,16 +3268,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D3">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="E3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F3">
         <v>2.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10.3</v>
       </c>
@@ -3294,19 +3282,16 @@
         <v>10.3</v>
       </c>
       <c r="C4">
-        <v>10.3</v>
+        <v>11.2</v>
       </c>
       <c r="D4">
-        <v>10.3</v>
+        <v>11.5</v>
       </c>
       <c r="E4">
-        <v>11.2</v>
-      </c>
-      <c r="F4">
         <v>11.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2.4</v>
       </c>
@@ -3314,19 +3299,16 @@
         <v>2.4</v>
       </c>
       <c r="C5">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D5">
         <v>2.4</v>
       </c>
       <c r="E5">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F5">
         <v>2.4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3342,11 +3324,8 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -3362,11 +3341,8 @@
       <c r="E7">
         <v>0.5</v>
       </c>
-      <c r="F7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6.9</v>
       </c>
@@ -3374,19 +3350,16 @@
         <v>6.9</v>
       </c>
       <c r="C8">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="D8">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="E8">
         <v>6.8</v>
       </c>
-      <c r="F8">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1.6</v>
       </c>
@@ -3397,16 +3370,13 @@
         <v>1.6</v>
       </c>
       <c r="D9">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E9">
-        <v>1.6</v>
-      </c>
-      <c r="F9">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7.6</v>
       </c>
@@ -3414,19 +3384,16 @@
         <v>7.6</v>
       </c>
       <c r="C10">
-        <v>7.6</v>
+        <v>7.4</v>
       </c>
       <c r="D10">
-        <v>7.6</v>
+        <v>7.3</v>
       </c>
       <c r="E10">
-        <v>7.4</v>
-      </c>
-      <c r="F10">
         <v>7.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3442,11 +3409,8 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3462,11 +3426,8 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3474,19 +3435,16 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E13">
-        <v>1.4</v>
-      </c>
-      <c r="F13">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1.5</v>
       </c>
@@ -3497,16 +3455,13 @@
         <v>1.5</v>
       </c>
       <c r="D14">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E14">
-        <v>1.5</v>
-      </c>
-      <c r="F14">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7.4</v>
       </c>
@@ -3514,19 +3469,16 @@
         <v>7.4</v>
       </c>
       <c r="C15">
-        <v>7.4</v>
+        <v>7.1</v>
       </c>
       <c r="D15">
-        <v>7.4</v>
+        <v>7.2</v>
       </c>
       <c r="E15">
-        <v>7.1</v>
-      </c>
-      <c r="F15">
         <v>7.2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3542,11 +3494,8 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3562,11 +3511,8 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -3582,11 +3528,8 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0</v>
       </c>
@@ -3600,9 +3543,6 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
         <v>0</v>
       </c>
     </row>

</xml_diff>